<commit_message>
have counties working now
</commit_message>
<xml_diff>
--- a/data/ma.xlsx
+++ b/data/ma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dd/gitcode/covid-compute/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462AD69F-DCD6-F04A-B1B7-331543A693D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506C49FB-C6F9-8C42-95CC-3970D88E083E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5260" yWindow="2940" windowWidth="32640" windowHeight="19100" xr2:uid="{CB30B321-1480-9C49-ACE9-CBB5D2FAF132}"/>
+    <workbookView xWindow="28440" yWindow="6240" windowWidth="32640" windowHeight="19100" xr2:uid="{CB30B321-1480-9C49-ACE9-CBB5D2FAF132}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -479,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ECAD043-FC09-3B43-BF4D-6B30E18A11C2}">
-  <dimension ref="A1:Z18"/>
+  <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y41" sqref="Y41"/>
+      <selection activeCell="W26" sqref="W26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -710,7 +710,7 @@
         <v>1839</v>
       </c>
       <c r="V4">
-        <f t="shared" ref="V4:V18" si="3">B4</f>
+        <f t="shared" ref="V4:V20" si="3">B4</f>
         <v>218</v>
       </c>
       <c r="W4">
@@ -739,7 +739,7 @@
         <v>256</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" ref="C5:C18" si="6">(B5-B4)/B4</f>
+        <f t="shared" ref="C5:C20" si="6">(B5-B4)/B4</f>
         <v>0.1743119266055046</v>
       </c>
       <c r="D5">
@@ -998,7 +998,7 @@
         <v>61</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" ref="F8:F18" si="13">E8/B8</f>
+        <f t="shared" ref="F8:F20" si="13">E8/B8</f>
         <v>0.11619047619047619</v>
       </c>
       <c r="G8">
@@ -1563,8 +1563,99 @@
         <v>0.20956059874456784</v>
       </c>
       <c r="Z18" s="2">
-        <f t="shared" ref="Z18" si="38">V18/U18</f>
+        <f t="shared" ref="Z18:Z20" si="38">V18/U18</f>
         <v>0.14104612762330884</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B19">
+        <v>7738</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="6"/>
+        <v>0.16888217522658611</v>
+      </c>
+      <c r="D19">
+        <v>122</v>
+      </c>
+      <c r="E19">
+        <v>682</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="13"/>
+        <v>8.8136469371930731E-2</v>
+      </c>
+      <c r="U19">
+        <v>51738</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="3"/>
+        <v>7738</v>
+      </c>
+      <c r="W19">
+        <f t="shared" ref="W19" si="39">U19-U18</f>
+        <v>4803</v>
+      </c>
+      <c r="X19">
+        <f t="shared" ref="X19" si="40">V19-V18</f>
+        <v>1118</v>
+      </c>
+      <c r="Y19" s="2">
+        <f t="shared" ref="Y19" si="41">X19/W19</f>
+        <v>0.23277118467624403</v>
+      </c>
+      <c r="Z19" s="2">
+        <f t="shared" si="38"/>
+        <v>0.14956125091808728</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <f>A19+1</f>
+        <v>43923</v>
+      </c>
+      <c r="B20">
+        <v>8966</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="6"/>
+        <v>0.15869733781338846</v>
+      </c>
+      <c r="D20">
+        <v>154</v>
+      </c>
+      <c r="E20">
+        <v>813</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="13"/>
+        <v>9.0675886683024759E-2</v>
+      </c>
+      <c r="U20">
+        <v>56608</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="3"/>
+        <v>8966</v>
+      </c>
+      <c r="W20">
+        <f t="shared" ref="W20" si="42">U20-U19</f>
+        <v>4870</v>
+      </c>
+      <c r="X20">
+        <f t="shared" ref="X20" si="43">V20-V19</f>
+        <v>1228</v>
+      </c>
+      <c r="Y20" s="2">
+        <f t="shared" ref="Y20" si="44">X20/W20</f>
+        <v>0.25215605749486653</v>
+      </c>
+      <c r="Z20" s="2">
+        <f t="shared" si="38"/>
+        <v>0.15838750706613905</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more state routines, updated data to 4/20
</commit_message>
<xml_diff>
--- a/data/ma.xlsx
+++ b/data/ma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dd/gitcode/covid-compute/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68B023F-913A-1341-BD35-A95BC0106ABD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F400AEF-91BA-3C40-98EC-BBED3F6D85CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31060" yWindow="5540" windowWidth="32640" windowHeight="19100" xr2:uid="{CB30B321-1480-9C49-ACE9-CBB5D2FAF132}"/>
+    <workbookView xWindow="42040" yWindow="2860" windowWidth="18180" windowHeight="19100" xr2:uid="{CB30B321-1480-9C49-ACE9-CBB5D2FAF132}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>Daily MA reports on COVID-19 from mass.gov website</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Tot pos rate</t>
+  </si>
+  <si>
+    <t>Death rate</t>
   </si>
 </sst>
 </file>
@@ -479,42 +482,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ECAD043-FC09-3B43-BF4D-6B30E18A11C2}">
-  <dimension ref="A1:AB22"/>
+  <dimension ref="A1:AC38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="Y38" sqref="Y38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.5" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" customWidth="1"/>
-    <col min="4" max="5" width="7.33203125" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" customWidth="1"/>
-    <col min="7" max="7" width="8.1640625" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" customWidth="1"/>
-    <col min="9" max="9" width="9" hidden="1" customWidth="1"/>
-    <col min="10" max="14" width="0" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="5.5" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="17" max="21" width="0.1640625" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="6" customWidth="1"/>
+    <col min="3" max="5" width="10.83203125" customWidth="1"/>
+    <col min="6" max="22" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="Q1" s="3" t="s">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="R1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="3"/>
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
       <c r="U1" s="3"/>
-      <c r="W1" t="s">
+      <c r="V1" s="3"/>
+      <c r="X1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -531,70 +526,73 @@
         <v>21</v>
       </c>
       <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>6</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>7</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>8</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>9</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>10</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="X2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43906</v>
       </c>
@@ -604,52 +602,52 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>14</v>
       </c>
-      <c r="H3" s="2">
-        <f>F3/B3</f>
+      <c r="I3" s="2">
+        <f>G3/B3</f>
         <v>7.1065989847715741E-2</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>1092</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>181</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>48</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>1</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>156</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>1</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>8</v>
       </c>
-      <c r="Q3">
-        <f>I3+K3+M3</f>
+      <c r="R3">
+        <f>J3+L3+N3</f>
         <v>1296</v>
       </c>
-      <c r="W3">
-        <f>Q3 + INT(O3/0.09)</f>
+      <c r="X3">
+        <f>R3 + INT(P3/0.09)</f>
         <v>1384</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <f>B3</f>
         <v>197</v>
       </c>
-      <c r="AB3" s="2">
-        <f>X3/W3</f>
+      <c r="AC3" s="2">
+        <f>Y3/X3</f>
         <v>0.14234104046242774</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <f>A3+1</f>
         <v>43907</v>
@@ -665,84 +663,85 @@
         <v>0</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4">
+      <c r="F4" s="2"/>
+      <c r="G4">
         <v>21</v>
       </c>
-      <c r="G4" s="2">
-        <f>(F4-F3)/F3</f>
+      <c r="H4" s="2">
+        <f>(G4-G3)/G3</f>
         <v>0.5</v>
       </c>
-      <c r="H4" s="2">
-        <f>F4/B4</f>
+      <c r="I4" s="2">
+        <f>G4/B4</f>
         <v>9.6330275229357804E-2</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1367</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>197</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>164</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>1</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>220</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>12</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>8</v>
       </c>
-      <c r="Q4">
-        <f t="shared" ref="Q4:Q7" si="0">I4+K4+M4</f>
+      <c r="R4">
+        <f t="shared" ref="R4:R7" si="0">J4+L4+N4</f>
         <v>1751</v>
       </c>
-      <c r="R4" s="2">
-        <f t="shared" ref="R4:R9" si="1">(B4-O4)/Q4</f>
+      <c r="S4" s="2">
+        <f t="shared" ref="S4:S9" si="1">(B4-P4)/R4</f>
         <v>0.11993146773272416</v>
       </c>
-      <c r="S4">
-        <f>Q4-Q3</f>
+      <c r="T4">
+        <f>R4-R3</f>
         <v>455</v>
       </c>
-      <c r="T4">
-        <f>B4-B3-(O4-O3)</f>
+      <c r="U4">
+        <f>B4-B3-(P4-P3)</f>
         <v>21</v>
       </c>
-      <c r="U4" s="2">
-        <f>T4/S4</f>
+      <c r="V4" s="2">
+        <f>U4/T4</f>
         <v>4.6153846153846156E-2</v>
       </c>
-      <c r="W4">
-        <f t="shared" ref="W4:W9" si="2">Q4 + INT(O4/0.09)</f>
+      <c r="X4">
+        <f t="shared" ref="X4:X9" si="2">R4 + INT(P4/0.09)</f>
         <v>1839</v>
       </c>
-      <c r="X4">
-        <f t="shared" ref="X4:X22" si="3">B4</f>
+      <c r="Y4">
+        <f t="shared" ref="Y4:Y24" si="3">B4</f>
         <v>218</v>
-      </c>
-      <c r="Y4">
-        <f>W4-W3</f>
-        <v>455</v>
       </c>
       <c r="Z4">
         <f>X4-X3</f>
+        <v>455</v>
+      </c>
+      <c r="AA4">
+        <f>Y4-Y3</f>
         <v>21</v>
       </c>
-      <c r="AA4" s="2">
-        <f>Z4/Y4</f>
+      <c r="AB4" s="2">
+        <f>AA4/Z4</f>
         <v>4.6153846153846156E-2</v>
       </c>
-      <c r="AB4" s="2">
-        <f t="shared" ref="AB4:AB11" si="4">X4/W4</f>
+      <c r="AC4" s="2">
+        <f t="shared" ref="AC4:AC11" si="4">Y4/X4</f>
         <v>0.11854268624252311</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A16" si="5">A4+1</f>
         <v>43908</v>
@@ -751,91 +750,92 @@
         <v>256</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" ref="C5:G22" si="6">(B5-B4)/B4</f>
+        <f t="shared" ref="C5:H31" si="6">(B5-B4)/B4</f>
         <v>0.1743119266055046</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5">
+      <c r="F5" s="2"/>
+      <c r="G5">
         <v>27</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <f t="shared" si="6"/>
         <v>0.2857142857142857</v>
       </c>
-      <c r="H5" s="2">
-        <f>F5/B5</f>
+      <c r="I5" s="2">
+        <f>G5/B5</f>
         <v>0.10546875</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>1743</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>224</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>306</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>11</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>222</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>12</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>9</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <f t="shared" si="0"/>
         <v>2271</v>
       </c>
-      <c r="R5" s="2">
+      <c r="S5" s="2">
         <f t="shared" si="1"/>
         <v>0.10876265962131219</v>
       </c>
-      <c r="S5">
-        <f t="shared" ref="S5:S9" si="7">Q5-Q4</f>
+      <c r="T5">
+        <f t="shared" ref="T5:T9" si="7">R5-R4</f>
         <v>520</v>
       </c>
-      <c r="T5">
-        <f t="shared" ref="T5:T8" si="8">B5-B4-(O5-O4)</f>
+      <c r="U5">
+        <f t="shared" ref="U5:U8" si="8">B5-B4-(P5-P4)</f>
         <v>37</v>
       </c>
-      <c r="U5" s="2">
-        <f t="shared" ref="U5:U8" si="9">T5/S5</f>
+      <c r="V5" s="2">
+        <f t="shared" ref="V5:V8" si="9">U5/T5</f>
         <v>7.1153846153846151E-2</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <f t="shared" si="2"/>
         <v>2371</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <f t="shared" si="3"/>
         <v>256</v>
       </c>
-      <c r="Y5">
-        <f t="shared" ref="Y5:Y9" si="10">W5-W4</f>
+      <c r="Z5">
+        <f t="shared" ref="Z5:Z9" si="10">X5-X4</f>
         <v>532</v>
       </c>
-      <c r="Z5">
-        <f t="shared" ref="Z5:Z9" si="11">X5-X4</f>
+      <c r="AA5">
+        <f t="shared" ref="AA5:AA9" si="11">Y5-Y4</f>
         <v>38</v>
       </c>
-      <c r="AA5" s="2">
-        <f t="shared" ref="AA5:AA10" si="12">Z5/Y5</f>
+      <c r="AB5" s="2">
+        <f t="shared" ref="AB5:AB10" si="12">AA5/Z5</f>
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="AB5" s="2">
+      <c r="AC5" s="2">
         <f t="shared" si="4"/>
         <v>0.10797132011809363</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <f t="shared" si="5"/>
         <v>43909</v>
@@ -851,84 +851,85 @@
         <v>0</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6">
+      <c r="F6" s="2"/>
+      <c r="G6">
         <v>43</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <f t="shared" si="6"/>
         <v>0.59259259259259256</v>
       </c>
-      <c r="H6" s="2">
-        <f>F6/B6</f>
+      <c r="I6" s="2">
+        <f>G6/B6</f>
         <v>0.13109756097560976</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>2208</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>261</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>699</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>29</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>225</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>12</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>26</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <f t="shared" si="0"/>
         <v>3132</v>
       </c>
-      <c r="R6" s="2">
+      <c r="S6" s="2">
         <f t="shared" si="1"/>
         <v>9.6424010217113665E-2</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <f t="shared" si="7"/>
         <v>861</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <f t="shared" si="8"/>
         <v>55</v>
       </c>
-      <c r="U6" s="2">
+      <c r="V6" s="2">
         <f t="shared" si="9"/>
         <v>6.3879210220673638E-2</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <f t="shared" si="2"/>
         <v>3420</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <f t="shared" si="3"/>
         <v>328</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <f t="shared" si="10"/>
         <v>1049</v>
       </c>
-      <c r="Z6">
+      <c r="AA6">
         <f t="shared" si="11"/>
         <v>72</v>
       </c>
-      <c r="AA6" s="2">
+      <c r="AB6" s="2">
         <f t="shared" si="12"/>
         <v>6.8636796949475692E-2</v>
       </c>
-      <c r="AB6" s="2">
+      <c r="AC6" s="2">
         <f t="shared" si="4"/>
         <v>9.5906432748538009E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <f t="shared" si="5"/>
         <v>43910</v>
@@ -944,66 +945,67 @@
         <v>1</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="F7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7">
+      <c r="I7" s="2"/>
+      <c r="J7">
         <v>2666</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>1039</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>485</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>40</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <f t="shared" si="0"/>
         <v>4190</v>
       </c>
-      <c r="R7" s="2">
+      <c r="S7" s="2">
         <f t="shared" si="1"/>
         <v>8.9021479713603816E-2</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <f t="shared" si="7"/>
         <v>1058</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <f t="shared" si="8"/>
         <v>71</v>
       </c>
-      <c r="U7" s="2">
+      <c r="V7" s="2">
         <f t="shared" si="9"/>
         <v>6.7107750472589794E-2</v>
       </c>
-      <c r="W7">
+      <c r="X7">
         <f t="shared" si="2"/>
         <v>4634</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <f t="shared" si="3"/>
         <v>413</v>
       </c>
-      <c r="Y7">
+      <c r="Z7">
         <f t="shared" si="10"/>
         <v>1214</v>
       </c>
-      <c r="Z7">
+      <c r="AA7">
         <f t="shared" si="11"/>
         <v>85</v>
       </c>
-      <c r="AA7" s="2">
+      <c r="AB7" s="2">
         <f t="shared" si="12"/>
         <v>7.0016474464579898E-2</v>
       </c>
-      <c r="AB7" s="2">
+      <c r="AC7" s="2">
         <f t="shared" si="4"/>
         <v>8.9123867069486398E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <f t="shared" si="5"/>
         <v>43911</v>
@@ -1022,81 +1024,85 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
+        <f>D8/B8</f>
+        <v>1.9047619047619048E-3</v>
+      </c>
+      <c r="G8">
         <v>61</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2">
-        <f t="shared" ref="H8:H22" si="13">F8/B8</f>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2">
+        <f t="shared" ref="I8:I28" si="13">G8/B8</f>
         <v>0.11619047619047619</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>3031</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>328</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>1433</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>72</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>743</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>55</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>70</v>
       </c>
-      <c r="Q8">
-        <f>I8+K8+M8</f>
+      <c r="R8">
+        <f>J8+L8+N8</f>
         <v>5207</v>
       </c>
-      <c r="R8" s="2">
+      <c r="S8" s="2">
         <f t="shared" si="1"/>
         <v>8.7382369886691E-2</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <f t="shared" si="7"/>
         <v>1017</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <f t="shared" si="8"/>
         <v>82</v>
       </c>
-      <c r="U8" s="2">
+      <c r="V8" s="2">
         <f t="shared" si="9"/>
         <v>8.0629301868239925E-2</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <f t="shared" si="2"/>
         <v>5984</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <f t="shared" si="3"/>
         <v>525</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <f t="shared" si="10"/>
         <v>1350</v>
       </c>
-      <c r="Z8">
+      <c r="AA8">
         <f t="shared" si="11"/>
         <v>112</v>
       </c>
-      <c r="AA8" s="2">
+      <c r="AB8" s="2">
         <f t="shared" si="12"/>
         <v>8.2962962962962961E-2</v>
       </c>
-      <c r="AB8" s="2">
+      <c r="AC8" s="2">
         <f t="shared" si="4"/>
         <v>8.7733957219251341E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <f t="shared" si="5"/>
         <v>43912</v>
@@ -1115,84 +1121,88 @@
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
+        <f t="shared" ref="F9:F27" si="14">D9/B9</f>
+        <v>7.7399380804953561E-3</v>
+      </c>
+      <c r="G9">
         <v>71</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <f t="shared" si="6"/>
         <v>0.16393442622950818</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <f t="shared" si="13"/>
         <v>0.10990712074303406</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>3403</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>362</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>1651</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>103</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>950</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>80</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>101</v>
       </c>
-      <c r="Q9">
-        <f>I9+K9+M9</f>
+      <c r="R9">
+        <f>J9+L9+N9</f>
         <v>6004</v>
       </c>
-      <c r="R9" s="2">
+      <c r="S9" s="2">
         <f t="shared" si="1"/>
         <v>9.0772818121252499E-2</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <f t="shared" si="7"/>
         <v>797</v>
       </c>
-      <c r="T9">
-        <f t="shared" ref="T9" si="14">B9-B8-(O9-O8)</f>
+      <c r="U9">
+        <f t="shared" ref="U9" si="15">B9-B8-(P9-P8)</f>
         <v>90</v>
       </c>
-      <c r="U9" s="2">
-        <f t="shared" ref="U9" si="15">T9/S9</f>
+      <c r="V9" s="2">
+        <f t="shared" ref="V9" si="16">U9/T9</f>
         <v>0.11292346298619825</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <f t="shared" si="2"/>
         <v>7126</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <f t="shared" si="3"/>
         <v>646</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <f t="shared" si="10"/>
         <v>1142</v>
       </c>
-      <c r="Z9">
+      <c r="AA9">
         <f t="shared" si="11"/>
         <v>121</v>
       </c>
-      <c r="AA9" s="2">
+      <c r="AB9" s="2">
         <f t="shared" si="12"/>
         <v>0.10595446584938704</v>
       </c>
-      <c r="AB9" s="2">
+      <c r="AC9" s="2">
         <f t="shared" si="4"/>
         <v>9.0653943306202633E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <f t="shared" si="5"/>
         <v>43913</v>
@@ -1211,42 +1221,46 @@
         <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
+        <f t="shared" si="14"/>
+        <v>1.1583011583011582E-2</v>
+      </c>
+      <c r="G10">
         <v>79</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <f t="shared" si="6"/>
         <v>0.11267605633802817</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I10" s="2">
         <f t="shared" si="13"/>
         <v>0.10167310167310167</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <v>8922</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <f t="shared" si="3"/>
         <v>777</v>
       </c>
-      <c r="Y10">
-        <f t="shared" ref="Y10:Z12" si="16">W10-W9</f>
+      <c r="Z10">
+        <f t="shared" ref="Z10:AA12" si="17">X10-X9</f>
         <v>1796</v>
       </c>
-      <c r="Z10">
-        <f t="shared" si="16"/>
+      <c r="AA10">
+        <f t="shared" si="17"/>
         <v>131</v>
       </c>
-      <c r="AA10" s="2">
+      <c r="AB10" s="2">
         <f t="shared" si="12"/>
         <v>7.2939866369710463E-2</v>
       </c>
-      <c r="AB10" s="2">
+      <c r="AC10" s="2">
         <f t="shared" si="4"/>
         <v>8.708809683927371E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <f t="shared" si="5"/>
         <v>43914</v>
@@ -1265,42 +1279,46 @@
         <f t="shared" si="6"/>
         <v>0.22222222222222221</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
+        <f t="shared" si="14"/>
+        <v>9.4909404659188953E-3</v>
+      </c>
+      <c r="G11">
         <v>94</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <f t="shared" si="6"/>
         <v>0.189873417721519</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I11" s="2">
         <f t="shared" si="13"/>
         <v>8.1104400345125102E-2</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <v>13749</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <f t="shared" si="3"/>
         <v>1159</v>
       </c>
-      <c r="Y11">
-        <f t="shared" si="16"/>
+      <c r="Z11">
+        <f t="shared" si="17"/>
         <v>4827</v>
       </c>
-      <c r="Z11">
-        <f t="shared" si="16"/>
+      <c r="AA11">
+        <f t="shared" si="17"/>
         <v>382</v>
       </c>
-      <c r="AA11" s="2">
-        <f t="shared" ref="AA11" si="17">Z11/Y11</f>
+      <c r="AB11" s="2">
+        <f t="shared" ref="AB11" si="18">AA11/Z11</f>
         <v>7.9138181064843591E-2</v>
       </c>
-      <c r="AB11" s="2">
+      <c r="AC11" s="2">
         <f t="shared" si="4"/>
         <v>8.4297039784711619E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <f t="shared" si="5"/>
         <v>43915</v>
@@ -1319,42 +1337,46 @@
         <f t="shared" si="6"/>
         <v>0.36363636363636365</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
+        <f t="shared" si="14"/>
+        <v>8.1610446137105556E-3</v>
+      </c>
+      <c r="G12">
         <v>103</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <f t="shared" si="6"/>
         <v>9.5744680851063829E-2</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I12" s="2">
         <f t="shared" si="13"/>
         <v>5.6039173014145807E-2</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <v>19794</v>
       </c>
-      <c r="X12">
+      <c r="Y12">
         <f t="shared" si="3"/>
         <v>1838</v>
       </c>
-      <c r="Y12">
-        <f t="shared" si="16"/>
+      <c r="Z12">
+        <f t="shared" si="17"/>
         <v>6045</v>
       </c>
-      <c r="Z12">
-        <f t="shared" si="16"/>
+      <c r="AA12">
+        <f t="shared" si="17"/>
         <v>679</v>
       </c>
-      <c r="AA12" s="2">
-        <f t="shared" ref="AA12" si="18">Z12/Y12</f>
+      <c r="AB12" s="2">
+        <f t="shared" ref="AB12" si="19">AA12/Z12</f>
         <v>0.11232423490488007</v>
       </c>
-      <c r="AB12" s="2">
-        <f t="shared" ref="AB12:AB17" si="19">X12/W12</f>
+      <c r="AC12" s="2">
+        <f t="shared" ref="AC12:AC17" si="20">Y12/X12</f>
         <v>9.2856421137718498E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <f t="shared" si="5"/>
         <v>43916</v>
@@ -1373,42 +1395,46 @@
         <f t="shared" si="6"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
+        <f t="shared" si="14"/>
+        <v>1.0343400910219279E-2</v>
+      </c>
+      <c r="G13">
         <v>219</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <f t="shared" si="6"/>
         <v>1.1262135922330097</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I13" s="2">
         <f t="shared" si="13"/>
         <v>9.0608191973520893E-2</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <v>23621</v>
       </c>
-      <c r="X13">
+      <c r="Y13">
         <f t="shared" si="3"/>
         <v>2417</v>
       </c>
-      <c r="Y13">
-        <f t="shared" ref="Y13" si="20">W13-W12</f>
-        <v>3827</v>
-      </c>
       <c r="Z13">
         <f t="shared" ref="Z13" si="21">X13-X12</f>
+        <v>3827</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" ref="AA13" si="22">Y13-Y12</f>
         <v>579</v>
       </c>
-      <c r="AA13" s="2">
-        <f t="shared" ref="AA13" si="22">Z13/Y13</f>
+      <c r="AB13" s="2">
+        <f t="shared" ref="AB13" si="23">AA13/Z13</f>
         <v>0.15129344133786254</v>
       </c>
-      <c r="AB13" s="2">
-        <f t="shared" si="19"/>
+      <c r="AC13" s="2">
+        <f t="shared" si="20"/>
         <v>0.10232420303966809</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <f t="shared" si="5"/>
         <v>43917</v>
@@ -1427,42 +1453,46 @@
         <f t="shared" si="6"/>
         <v>0.4</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
+        <f t="shared" si="14"/>
+        <v>1.0802469135802469E-2</v>
+      </c>
+      <c r="G14">
         <v>288</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="2">
         <f t="shared" si="6"/>
         <v>0.31506849315068491</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I14" s="2">
         <f t="shared" si="13"/>
         <v>8.8888888888888892E-2</v>
       </c>
-      <c r="W14">
+      <c r="X14">
         <v>29371</v>
       </c>
-      <c r="X14">
+      <c r="Y14">
         <f t="shared" si="3"/>
         <v>3240</v>
       </c>
-      <c r="Y14">
-        <f t="shared" ref="Y14" si="23">W14-W13</f>
-        <v>5750</v>
-      </c>
       <c r="Z14">
         <f t="shared" ref="Z14" si="24">X14-X13</f>
+        <v>5750</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" ref="AA14" si="25">Y14-Y13</f>
         <v>823</v>
       </c>
-      <c r="AA14" s="2">
-        <f t="shared" ref="AA14" si="25">Z14/Y14</f>
+      <c r="AB14" s="2">
+        <f t="shared" ref="AB14" si="26">AA14/Z14</f>
         <v>0.1431304347826087</v>
       </c>
-      <c r="AB14" s="2">
-        <f t="shared" si="19"/>
+      <c r="AC14" s="2">
+        <f t="shared" si="20"/>
         <v>0.11031289367062749</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <f t="shared" si="5"/>
         <v>43918</v>
@@ -1481,42 +1511,46 @@
         <f t="shared" si="6"/>
         <v>0.25714285714285712</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
+        <f t="shared" si="14"/>
+        <v>1.0335917312661499E-2</v>
+      </c>
+      <c r="G15">
         <v>350</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <f t="shared" si="6"/>
         <v>0.21527777777777779</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <f t="shared" si="13"/>
         <v>8.2217524077989199E-2</v>
       </c>
-      <c r="W15">
+      <c r="X15">
         <v>35049</v>
       </c>
-      <c r="X15">
+      <c r="Y15">
         <f t="shared" si="3"/>
         <v>4257</v>
       </c>
-      <c r="Y15">
-        <f t="shared" ref="Y15" si="26">W15-W14</f>
-        <v>5678</v>
-      </c>
       <c r="Z15">
         <f t="shared" ref="Z15" si="27">X15-X14</f>
+        <v>5678</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" ref="AA15" si="28">Y15-Y14</f>
         <v>1017</v>
       </c>
-      <c r="AA15" s="2">
-        <f t="shared" ref="AA15" si="28">Z15/Y15</f>
+      <c r="AB15" s="2">
+        <f t="shared" ref="AB15" si="29">AA15/Z15</f>
         <v>0.17911236350827756</v>
       </c>
-      <c r="AB15" s="2">
-        <f t="shared" si="19"/>
+      <c r="AC15" s="2">
+        <f t="shared" si="20"/>
         <v>0.12145852948728922</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <f t="shared" si="5"/>
         <v>43919</v>
@@ -1535,42 +1569,46 @@
         <f t="shared" si="6"/>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
+        <f t="shared" si="14"/>
+        <v>9.6871846619576187E-3</v>
+      </c>
+      <c r="G16">
         <v>399</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <f t="shared" si="6"/>
         <v>0.14000000000000001</v>
       </c>
-      <c r="H16" s="2">
+      <c r="I16" s="2">
         <f t="shared" si="13"/>
         <v>8.0524722502522711E-2</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <v>39066</v>
       </c>
-      <c r="X16">
+      <c r="Y16">
         <f t="shared" si="3"/>
         <v>4955</v>
       </c>
-      <c r="Y16">
-        <f t="shared" ref="Y16" si="29">W16-W15</f>
-        <v>4017</v>
-      </c>
       <c r="Z16">
         <f t="shared" ref="Z16" si="30">X16-X15</f>
+        <v>4017</v>
+      </c>
+      <c r="AA16">
+        <f t="shared" ref="AA16" si="31">Y16-Y15</f>
         <v>698</v>
       </c>
-      <c r="AA16" s="2">
-        <f t="shared" ref="AA16" si="31">Z16/Y16</f>
+      <c r="AB16" s="2">
+        <f t="shared" ref="AB16" si="32">AA16/Z16</f>
         <v>0.17376151356733882</v>
       </c>
-      <c r="AB16" s="2">
-        <f t="shared" si="19"/>
+      <c r="AC16" s="2">
+        <f t="shared" si="20"/>
         <v>0.12683663543746479</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43920</v>
       </c>
@@ -1588,42 +1626,46 @@
         <f t="shared" si="6"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
+        <f t="shared" si="14"/>
+        <v>9.7357440890125171E-3</v>
+      </c>
+      <c r="G17">
         <v>453</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <f t="shared" si="6"/>
         <v>0.13533834586466165</v>
       </c>
-      <c r="H17" s="2">
+      <c r="I17" s="2">
         <f t="shared" si="13"/>
         <v>7.8755215577190549E-2</v>
       </c>
-      <c r="W17">
+      <c r="X17">
         <v>42793</v>
       </c>
-      <c r="X17">
+      <c r="Y17">
         <f t="shared" si="3"/>
         <v>5752</v>
       </c>
-      <c r="Y17">
-        <f t="shared" ref="Y17" si="32">W17-W16</f>
-        <v>3727</v>
-      </c>
       <c r="Z17">
         <f t="shared" ref="Z17" si="33">X17-X16</f>
+        <v>3727</v>
+      </c>
+      <c r="AA17">
+        <f t="shared" ref="AA17" si="34">Y17-Y16</f>
         <v>797</v>
       </c>
-      <c r="AA17" s="2">
-        <f t="shared" ref="AA17" si="34">Z17/Y17</f>
+      <c r="AB17" s="2">
+        <f t="shared" ref="AB17" si="35">AA17/Z17</f>
         <v>0.2138449154816206</v>
       </c>
-      <c r="AB17" s="2">
-        <f t="shared" si="19"/>
+      <c r="AC17" s="2">
+        <f t="shared" si="20"/>
         <v>0.13441450704554483</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43921</v>
       </c>
@@ -1641,42 +1683,46 @@
         <f t="shared" si="6"/>
         <v>0.5892857142857143</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
+        <f t="shared" si="14"/>
+        <v>1.3444108761329305E-2</v>
+      </c>
+      <c r="G18">
         <v>562</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H18" s="2">
         <f t="shared" si="6"/>
         <v>0.24061810154525387</v>
       </c>
-      <c r="H18" s="2">
+      <c r="I18" s="2">
         <f t="shared" si="13"/>
         <v>8.4894259818731124E-2</v>
       </c>
-      <c r="W18">
+      <c r="X18">
         <v>46935</v>
       </c>
-      <c r="X18">
+      <c r="Y18">
         <f t="shared" si="3"/>
         <v>6620</v>
       </c>
-      <c r="Y18">
-        <f t="shared" ref="Y18" si="35">W18-W17</f>
-        <v>4142</v>
-      </c>
       <c r="Z18">
         <f t="shared" ref="Z18" si="36">X18-X17</f>
+        <v>4142</v>
+      </c>
+      <c r="AA18">
+        <f t="shared" ref="AA18" si="37">Y18-Y17</f>
         <v>868</v>
       </c>
-      <c r="AA18" s="2">
-        <f t="shared" ref="AA18" si="37">Z18/Y18</f>
+      <c r="AB18" s="2">
+        <f t="shared" ref="AB18" si="38">AA18/Z18</f>
         <v>0.20956059874456784</v>
       </c>
-      <c r="AB18" s="2">
-        <f t="shared" ref="AB18:AB20" si="38">X18/W18</f>
+      <c r="AC18" s="2">
+        <f t="shared" ref="AC18:AC20" si="39">Y18/X18</f>
         <v>0.14104612762330884</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43922</v>
       </c>
@@ -1694,44 +1740,48 @@
         <f t="shared" si="6"/>
         <v>0.3707865168539326</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
+        <f t="shared" si="14"/>
+        <v>1.5766347893512535E-2</v>
+      </c>
+      <c r="G19">
         <v>682</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H19" s="2">
         <f t="shared" si="6"/>
         <v>0.21352313167259787</v>
       </c>
-      <c r="H19" s="2">
+      <c r="I19" s="2">
         <f t="shared" si="13"/>
         <v>8.8136469371930731E-2</v>
       </c>
-      <c r="W19">
+      <c r="X19">
         <v>51738</v>
       </c>
-      <c r="X19">
+      <c r="Y19">
         <f t="shared" si="3"/>
         <v>7738</v>
       </c>
-      <c r="Y19">
-        <f t="shared" ref="Y19" si="39">W19-W18</f>
-        <v>4803</v>
-      </c>
       <c r="Z19">
         <f t="shared" ref="Z19" si="40">X19-X18</f>
+        <v>4803</v>
+      </c>
+      <c r="AA19">
+        <f t="shared" ref="AA19" si="41">Y19-Y18</f>
         <v>1118</v>
       </c>
-      <c r="AA19" s="2">
-        <f t="shared" ref="AA19" si="41">Z19/Y19</f>
+      <c r="AB19" s="2">
+        <f t="shared" ref="AB19" si="42">AA19/Z19</f>
         <v>0.23277118467624403</v>
       </c>
-      <c r="AB19" s="2">
-        <f t="shared" si="38"/>
+      <c r="AC19" s="2">
+        <f t="shared" si="39"/>
         <v>0.14956125091808728</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <f>A19+1</f>
+        <f t="shared" ref="A20:A38" si="43">A19+1</f>
         <v>43923</v>
       </c>
       <c r="B20">
@@ -1748,44 +1798,48 @@
         <f t="shared" si="6"/>
         <v>0.26229508196721313</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
+        <f t="shared" si="14"/>
+        <v>1.7175998215480704E-2</v>
+      </c>
+      <c r="G20">
         <v>813</v>
       </c>
-      <c r="G20" s="2">
+      <c r="H20" s="2">
         <f t="shared" si="6"/>
         <v>0.19208211143695014</v>
       </c>
-      <c r="H20" s="2">
+      <c r="I20" s="2">
         <f t="shared" si="13"/>
         <v>9.0675886683024759E-2</v>
       </c>
-      <c r="W20">
+      <c r="X20">
         <v>56608</v>
       </c>
-      <c r="X20">
+      <c r="Y20">
         <f t="shared" si="3"/>
         <v>8966</v>
       </c>
-      <c r="Y20">
-        <f t="shared" ref="Y20" si="42">W20-W19</f>
+      <c r="Z20">
+        <f t="shared" ref="Z20" si="44">X20-X19</f>
         <v>4870</v>
       </c>
-      <c r="Z20">
-        <f t="shared" ref="Z20" si="43">X20-X19</f>
+      <c r="AA20">
+        <f t="shared" ref="AA20" si="45">Y20-Y19</f>
         <v>1228</v>
       </c>
-      <c r="AA20" s="2">
-        <f t="shared" ref="AA20" si="44">Z20/Y20</f>
+      <c r="AB20" s="2">
+        <f t="shared" ref="AB20" si="46">AA20/Z20</f>
         <v>0.25215605749486653</v>
       </c>
-      <c r="AB20" s="2">
-        <f t="shared" si="38"/>
+      <c r="AC20" s="2">
+        <f t="shared" si="39"/>
         <v>0.15838750706613905</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <f>A20+1</f>
+        <f t="shared" si="43"/>
         <v>43924</v>
       </c>
       <c r="B21">
@@ -1802,44 +1856,48 @@
         <f t="shared" si="6"/>
         <v>0.24675324675324675</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
+        <f t="shared" si="14"/>
+        <v>1.8457988848298405E-2</v>
+      </c>
+      <c r="G21">
         <v>966</v>
       </c>
-      <c r="G21" s="2">
+      <c r="H21" s="2">
         <f t="shared" si="6"/>
         <v>0.18819188191881919</v>
       </c>
-      <c r="H21" s="2">
+      <c r="I21" s="2">
         <f t="shared" si="13"/>
         <v>9.2866756393001348E-2</v>
       </c>
-      <c r="W21">
+      <c r="X21">
         <v>62962</v>
       </c>
-      <c r="X21">
+      <c r="Y21">
         <f t="shared" si="3"/>
         <v>10402</v>
       </c>
-      <c r="Y21">
-        <f t="shared" ref="Y21" si="45">W21-W20</f>
+      <c r="Z21">
+        <f t="shared" ref="Z21" si="47">X21-X20</f>
         <v>6354</v>
       </c>
-      <c r="Z21">
-        <f t="shared" ref="Z21" si="46">X21-X20</f>
+      <c r="AA21">
+        <f t="shared" ref="AA21" si="48">Y21-Y20</f>
         <v>1436</v>
       </c>
-      <c r="AA21" s="2">
-        <f t="shared" ref="AA21" si="47">Z21/Y21</f>
+      <c r="AB21" s="2">
+        <f t="shared" ref="AB21" si="49">AA21/Z21</f>
         <v>0.22599937047529114</v>
       </c>
-      <c r="AB21" s="2">
-        <f t="shared" ref="AB21:AB22" si="48">X21/W21</f>
+      <c r="AC21" s="2">
+        <f t="shared" ref="AC21:AC22" si="50">Y21/X21</f>
         <v>0.16521076204694896</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <f>A21+1</f>
+        <f t="shared" si="43"/>
         <v>43925</v>
       </c>
       <c r="B22">
@@ -1856,39 +1914,935 @@
         <f t="shared" si="6"/>
         <v>0.125</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
+        <f t="shared" si="14"/>
+        <v>1.8404907975460124E-2</v>
+      </c>
+      <c r="G22">
         <v>1068</v>
       </c>
-      <c r="G22" s="2">
+      <c r="H22" s="2">
         <f t="shared" si="6"/>
         <v>0.10559006211180125</v>
       </c>
-      <c r="H22" s="2">
+      <c r="I22" s="2">
         <f t="shared" si="13"/>
         <v>9.1002044989775058E-2</v>
       </c>
-      <c r="W22">
+      <c r="X22">
         <v>68800</v>
       </c>
-      <c r="X22">
+      <c r="Y22">
         <f t="shared" si="3"/>
         <v>11736</v>
       </c>
-      <c r="Y22">
-        <f t="shared" ref="Y22" si="49">W22-W21</f>
+      <c r="Z22">
+        <f t="shared" ref="Z22" si="51">X22-X21</f>
         <v>5838</v>
       </c>
-      <c r="Z22">
-        <f t="shared" ref="Z22" si="50">X22-X21</f>
+      <c r="AA22">
+        <f t="shared" ref="AA22" si="52">Y22-Y21</f>
         <v>1334</v>
       </c>
-      <c r="AA22" s="2">
-        <f t="shared" ref="AA22" si="51">Z22/Y22</f>
+      <c r="AB22" s="2">
+        <f t="shared" ref="AB22" si="53">AA22/Z22</f>
         <v>0.22850291195614936</v>
       </c>
-      <c r="AB22" s="2">
-        <f t="shared" si="48"/>
+      <c r="AC22" s="2">
+        <f t="shared" si="50"/>
         <v>0.17058139534883721</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <f t="shared" si="43"/>
+        <v>43926</v>
+      </c>
+      <c r="B23">
+        <v>12500</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="6"/>
+        <v>6.50988411724608E-2</v>
+      </c>
+      <c r="D23">
+        <v>231</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="6"/>
+        <v>6.9444444444444448E-2</v>
+      </c>
+      <c r="F23" s="2">
+        <f t="shared" si="14"/>
+        <v>1.848E-2</v>
+      </c>
+      <c r="G23">
+        <v>1145</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="6"/>
+        <v>7.2097378277153554E-2</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="13"/>
+        <v>9.1600000000000001E-2</v>
+      </c>
+      <c r="X23">
+        <v>71937</v>
+      </c>
+      <c r="Y23">
+        <f t="shared" si="3"/>
+        <v>12500</v>
+      </c>
+      <c r="Z23">
+        <f t="shared" ref="Z23" si="54">X23-X22</f>
+        <v>3137</v>
+      </c>
+      <c r="AA23">
+        <f t="shared" ref="AA23" si="55">Y23-Y22</f>
+        <v>764</v>
+      </c>
+      <c r="AB23" s="2">
+        <f t="shared" ref="AB23" si="56">AA23/Z23</f>
+        <v>0.24354478801402615</v>
+      </c>
+      <c r="AC23" s="2">
+        <f t="shared" ref="AC23:AC24" si="57">Y23/X23</f>
+        <v>0.17376315387074801</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <f t="shared" si="43"/>
+        <v>43927</v>
+      </c>
+      <c r="B24">
+        <v>13837</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="6"/>
+        <v>0.10696</v>
+      </c>
+      <c r="D24">
+        <v>280</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="6"/>
+        <v>0.21212121212121213</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" si="14"/>
+        <v>2.0235600202356003E-2</v>
+      </c>
+      <c r="G24">
+        <v>1241</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="6"/>
+        <v>8.3842794759825326E-2</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="13"/>
+        <v>8.968707089687071E-2</v>
+      </c>
+      <c r="X24">
+        <v>76429</v>
+      </c>
+      <c r="Y24">
+        <f t="shared" si="3"/>
+        <v>13837</v>
+      </c>
+      <c r="Z24">
+        <f t="shared" ref="Z24" si="58">X24-X23</f>
+        <v>4492</v>
+      </c>
+      <c r="AA24">
+        <f t="shared" ref="AA24" si="59">Y24-Y23</f>
+        <v>1337</v>
+      </c>
+      <c r="AB24" s="2">
+        <f t="shared" ref="AB24" si="60">AA24/Z24</f>
+        <v>0.29764024933214606</v>
+      </c>
+      <c r="AC24" s="2">
+        <f t="shared" si="57"/>
+        <v>0.18104384461395542</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <f t="shared" si="43"/>
+        <v>43928</v>
+      </c>
+      <c r="B25">
+        <v>15202</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="6"/>
+        <v>9.8648550986485506E-2</v>
+      </c>
+      <c r="D25">
+        <v>356</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="6"/>
+        <v>0.27142857142857141</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" si="14"/>
+        <v>2.3417971319563215E-2</v>
+      </c>
+      <c r="G25">
+        <v>1435</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="6"/>
+        <v>0.1563255439161966</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="13"/>
+        <v>9.4395474279700034E-2</v>
+      </c>
+      <c r="X25">
+        <v>81344</v>
+      </c>
+      <c r="Y25">
+        <f t="shared" ref="Y25:Y27" si="61">B25</f>
+        <v>15202</v>
+      </c>
+      <c r="Z25">
+        <f t="shared" ref="Z25" si="62">X25-X24</f>
+        <v>4915</v>
+      </c>
+      <c r="AA25">
+        <f t="shared" ref="AA25" si="63">Y25-Y24</f>
+        <v>1365</v>
+      </c>
+      <c r="AB25" s="2">
+        <f t="shared" ref="AB25" si="64">AA25/Z25</f>
+        <v>0.2777212614445575</v>
+      </c>
+      <c r="AC25" s="2">
+        <f t="shared" ref="AC25:AC27" si="65">Y25/X25</f>
+        <v>0.18688532651455547</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <f t="shared" si="43"/>
+        <v>43929</v>
+      </c>
+      <c r="B26">
+        <v>16790</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="6"/>
+        <v>0.10445993948164715</v>
+      </c>
+      <c r="D26">
+        <v>433</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="6"/>
+        <v>0.21629213483146068</v>
+      </c>
+      <c r="F26" s="2">
+        <f t="shared" si="14"/>
+        <v>2.578916021441334E-2</v>
+      </c>
+      <c r="G26">
+        <v>1583</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="6"/>
+        <v>0.10313588850174216</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="13"/>
+        <v>9.4282310899344843E-2</v>
+      </c>
+      <c r="X26">
+        <v>87511</v>
+      </c>
+      <c r="Y26">
+        <f t="shared" si="61"/>
+        <v>16790</v>
+      </c>
+      <c r="Z26">
+        <f t="shared" ref="Z26" si="66">X26-X25</f>
+        <v>6167</v>
+      </c>
+      <c r="AA26">
+        <f t="shared" ref="AA26" si="67">Y26-Y25</f>
+        <v>1588</v>
+      </c>
+      <c r="AB26" s="2">
+        <f t="shared" ref="AB26" si="68">AA26/Z26</f>
+        <v>0.25749959461650723</v>
+      </c>
+      <c r="AC26" s="2">
+        <f t="shared" si="65"/>
+        <v>0.19186159454240037</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <f t="shared" si="43"/>
+        <v>43930</v>
+      </c>
+      <c r="B27">
+        <v>18941</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" si="6"/>
+        <v>0.1281119714115545</v>
+      </c>
+      <c r="D27">
+        <v>503</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="6"/>
+        <v>0.16166281755196305</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" si="14"/>
+        <v>2.6556148038646324E-2</v>
+      </c>
+      <c r="G27">
+        <v>1747</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="6"/>
+        <v>0.10360075805432722</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="13"/>
+        <v>9.2233778575576797E-2</v>
+      </c>
+      <c r="X27">
+        <v>94978</v>
+      </c>
+      <c r="Y27">
+        <f t="shared" si="61"/>
+        <v>18941</v>
+      </c>
+      <c r="Z27">
+        <f t="shared" ref="Z27" si="69">X27-X26</f>
+        <v>7467</v>
+      </c>
+      <c r="AA27">
+        <f t="shared" ref="AA27" si="70">Y27-Y26</f>
+        <v>2151</v>
+      </c>
+      <c r="AB27" s="2">
+        <f t="shared" ref="AB27" si="71">AA27/Z27</f>
+        <v>0.28806749698674167</v>
+      </c>
+      <c r="AC27" s="2">
+        <f t="shared" si="65"/>
+        <v>0.19942513003011222</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <f t="shared" si="43"/>
+        <v>43931</v>
+      </c>
+      <c r="B28">
+        <f>20974</f>
+        <v>20974</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="6"/>
+        <v>0.10733329813631803</v>
+      </c>
+      <c r="D28">
+        <v>599</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" ref="E28" si="72">(D28-D27)/D27</f>
+        <v>0.19085487077534791</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" ref="F28" si="73">D28/B28</f>
+        <v>2.8559168494326308E-2</v>
+      </c>
+      <c r="G28">
+        <v>1956</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="6"/>
+        <v>0.11963365769891242</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="13"/>
+        <v>9.3258319824544675E-2</v>
+      </c>
+      <c r="X28">
+        <v>102372</v>
+      </c>
+      <c r="Y28">
+        <f t="shared" ref="Y28" si="74">B28</f>
+        <v>20974</v>
+      </c>
+      <c r="Z28">
+        <f t="shared" ref="Z28" si="75">X28-X27</f>
+        <v>7394</v>
+      </c>
+      <c r="AA28">
+        <f t="shared" ref="AA28" si="76">Y28-Y27</f>
+        <v>2033</v>
+      </c>
+      <c r="AB28" s="2">
+        <f t="shared" ref="AB28" si="77">AA28/Z28</f>
+        <v>0.2749526643224236</v>
+      </c>
+      <c r="AC28" s="2">
+        <f t="shared" ref="AC28" si="78">Y28/X28</f>
+        <v>0.2048802406908139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <f t="shared" si="43"/>
+        <v>43932</v>
+      </c>
+      <c r="B29">
+        <v>22860</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" si="6"/>
+        <v>8.9920854391150953E-2</v>
+      </c>
+      <c r="D29">
+        <v>686</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" ref="E29" si="79">(D29-D28)/D28</f>
+        <v>0.14524207011686144</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" ref="F29" si="80">D29/B29</f>
+        <v>3.00087489063867E-2</v>
+      </c>
+      <c r="G29">
+        <v>2120</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" ref="H29" si="81">(G29-G28)/G28</f>
+        <v>8.3844580777096112E-2</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" ref="I29" si="82">G29/B29</f>
+        <v>9.2738407699037614E-2</v>
+      </c>
+      <c r="X29">
+        <v>108776</v>
+      </c>
+      <c r="Y29">
+        <f t="shared" ref="Y29:Y38" si="83">B29</f>
+        <v>22860</v>
+      </c>
+      <c r="Z29">
+        <f t="shared" ref="Z29" si="84">X29-X28</f>
+        <v>6404</v>
+      </c>
+      <c r="AA29">
+        <f t="shared" ref="AA29" si="85">Y29-Y28</f>
+        <v>1886</v>
+      </c>
+      <c r="AB29" s="2">
+        <f t="shared" ref="AB29" si="86">AA29/Z29</f>
+        <v>0.29450343535290441</v>
+      </c>
+      <c r="AC29" s="2">
+        <f t="shared" ref="AC29" si="87">Y29/X29</f>
+        <v>0.21015665220269178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <f t="shared" si="43"/>
+        <v>43933</v>
+      </c>
+      <c r="B30">
+        <v>25475</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="6"/>
+        <v>0.11439195100612423</v>
+      </c>
+      <c r="D30">
+        <v>756</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" ref="E30" si="88">(D30-D29)/D29</f>
+        <v>0.10204081632653061</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" ref="F30" si="89">D30/B30</f>
+        <v>2.9676153091265946E-2</v>
+      </c>
+      <c r="G30">
+        <v>2235</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" ref="H30" si="90">(G30-G29)/G29</f>
+        <v>5.4245283018867926E-2</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" ref="I30" si="91">G30/B30</f>
+        <v>8.7733071638861626E-2</v>
+      </c>
+      <c r="X30">
+        <v>116730</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" si="83"/>
+        <v>25475</v>
+      </c>
+      <c r="Z30">
+        <f t="shared" ref="Z30" si="92">X30-X29</f>
+        <v>7954</v>
+      </c>
+      <c r="AA30">
+        <f t="shared" ref="AA30" si="93">Y30-Y29</f>
+        <v>2615</v>
+      </c>
+      <c r="AB30" s="2">
+        <f t="shared" ref="AB30" si="94">AA30/Z30</f>
+        <v>0.32876540105607244</v>
+      </c>
+      <c r="AC30" s="2">
+        <f t="shared" ref="AC30" si="95">Y30/X30</f>
+        <v>0.218238670436049</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <f t="shared" si="43"/>
+        <v>43934</v>
+      </c>
+      <c r="B31">
+        <v>26867</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="6"/>
+        <v>5.4641805691854763E-2</v>
+      </c>
+      <c r="D31">
+        <v>844</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" ref="E31:E38" si="96">(D31-D30)/D30</f>
+        <v>0.1164021164021164</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" ref="F31:F38" si="97">D31/B31</f>
+        <v>3.1414002307663676E-2</v>
+      </c>
+      <c r="G31">
+        <v>2340</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" ref="H31:H34" si="98">(G31-G30)/G30</f>
+        <v>4.6979865771812082E-2</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" ref="I31:I38" si="99">G31/B31</f>
+        <v>8.7095693601816349E-2</v>
+      </c>
+      <c r="X31">
+        <v>122049</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" si="83"/>
+        <v>26867</v>
+      </c>
+      <c r="Z31">
+        <f t="shared" ref="Z31:Z34" si="100">X31-X30</f>
+        <v>5319</v>
+      </c>
+      <c r="AA31">
+        <f t="shared" ref="AA31:AA34" si="101">Y31-Y30</f>
+        <v>1392</v>
+      </c>
+      <c r="AB31" s="2">
+        <f t="shared" ref="AB31:AB34" si="102">AA31/Z31</f>
+        <v>0.26170332769317539</v>
+      </c>
+      <c r="AC31" s="2">
+        <f t="shared" ref="AC31:AC37" si="103">Y31/X31</f>
+        <v>0.22013289744283035</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <f t="shared" si="43"/>
+        <v>43935</v>
+      </c>
+      <c r="B32">
+        <v>28163</v>
+      </c>
+      <c r="C32" s="2">
+        <f t="shared" ref="C32:C38" si="104">(B32-B31)/B31</f>
+        <v>4.8237614917929057E-2</v>
+      </c>
+      <c r="D32">
+        <v>957</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="96"/>
+        <v>0.13388625592417061</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="97"/>
+        <v>3.3980754891169265E-2</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="98"/>
+        <v>-1</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="X32">
+        <v>126551</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="83"/>
+        <v>28163</v>
+      </c>
+      <c r="Z32">
+        <f t="shared" si="100"/>
+        <v>4502</v>
+      </c>
+      <c r="AA32">
+        <f t="shared" si="101"/>
+        <v>1296</v>
+      </c>
+      <c r="AB32" s="2">
+        <f t="shared" si="102"/>
+        <v>0.28787205686361617</v>
+      </c>
+      <c r="AC32" s="2">
+        <f t="shared" si="103"/>
+        <v>0.22254269029877283</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <f t="shared" si="43"/>
+        <v>43936</v>
+      </c>
+      <c r="B33">
+        <v>29918</v>
+      </c>
+      <c r="C33" s="2">
+        <f t="shared" si="104"/>
+        <v>6.2315804424244579E-2</v>
+      </c>
+      <c r="D33">
+        <v>1108</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="96"/>
+        <v>0.15778474399164055</v>
+      </c>
+      <c r="F33" s="2">
+        <f t="shared" si="97"/>
+        <v>3.7034561133765624E-2</v>
+      </c>
+      <c r="H33" s="2" t="e">
+        <f t="shared" si="98"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="X33">
+        <v>132023</v>
+      </c>
+      <c r="Y33">
+        <f t="shared" si="83"/>
+        <v>29918</v>
+      </c>
+      <c r="Z33">
+        <f t="shared" si="100"/>
+        <v>5472</v>
+      </c>
+      <c r="AA33">
+        <f t="shared" si="101"/>
+        <v>1755</v>
+      </c>
+      <c r="AB33" s="2">
+        <f t="shared" si="102"/>
+        <v>0.32072368421052633</v>
+      </c>
+      <c r="AC33" s="2">
+        <f t="shared" si="103"/>
+        <v>0.22661202972209388</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <f t="shared" si="43"/>
+        <v>43937</v>
+      </c>
+      <c r="B34">
+        <v>32181</v>
+      </c>
+      <c r="C34" s="2">
+        <f t="shared" si="104"/>
+        <v>7.5640082893241534E-2</v>
+      </c>
+      <c r="D34">
+        <v>1245</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="96"/>
+        <v>0.12364620938628158</v>
+      </c>
+      <c r="F34" s="2">
+        <f t="shared" si="97"/>
+        <v>3.8687424256548898E-2</v>
+      </c>
+      <c r="H34" s="2" t="e">
+        <f t="shared" si="98"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="X34">
+        <v>140773</v>
+      </c>
+      <c r="Y34">
+        <f t="shared" si="83"/>
+        <v>32181</v>
+      </c>
+      <c r="Z34">
+        <f t="shared" si="100"/>
+        <v>8750</v>
+      </c>
+      <c r="AA34">
+        <f t="shared" si="101"/>
+        <v>2263</v>
+      </c>
+      <c r="AB34" s="2">
+        <f t="shared" si="102"/>
+        <v>0.25862857142857143</v>
+      </c>
+      <c r="AC34" s="2">
+        <f t="shared" si="103"/>
+        <v>0.22860207568212654</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <f t="shared" si="43"/>
+        <v>43938</v>
+      </c>
+      <c r="B35">
+        <v>34402</v>
+      </c>
+      <c r="C35" s="2">
+        <f t="shared" si="104"/>
+        <v>6.9015878934775177E-2</v>
+      </c>
+      <c r="D35">
+        <v>1404</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="96"/>
+        <v>0.12771084337349398</v>
+      </c>
+      <c r="F35" s="2">
+        <f t="shared" si="97"/>
+        <v>4.0811580722051044E-2</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="X35">
+        <v>148744</v>
+      </c>
+      <c r="Y35">
+        <f t="shared" si="83"/>
+        <v>34402</v>
+      </c>
+      <c r="Z35">
+        <f t="shared" ref="Z35" si="105">X35-X34</f>
+        <v>7971</v>
+      </c>
+      <c r="AA35">
+        <f t="shared" ref="AA35" si="106">Y35-Y34</f>
+        <v>2221</v>
+      </c>
+      <c r="AB35" s="2">
+        <f t="shared" ref="AB35" si="107">AA35/Z35</f>
+        <v>0.27863505206373101</v>
+      </c>
+      <c r="AC35" s="2">
+        <f t="shared" si="103"/>
+        <v>0.2312832786532566</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <f t="shared" si="43"/>
+        <v>43939</v>
+      </c>
+      <c r="B36">
+        <v>36372</v>
+      </c>
+      <c r="C36" s="2">
+        <f t="shared" si="104"/>
+        <v>5.7264112551595837E-2</v>
+      </c>
+      <c r="D36">
+        <v>1560</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="96"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="F36" s="2">
+        <f t="shared" si="97"/>
+        <v>4.2890135268888158E-2</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="X36">
+        <v>156806</v>
+      </c>
+      <c r="Y36">
+        <f t="shared" si="83"/>
+        <v>36372</v>
+      </c>
+      <c r="Z36">
+        <f t="shared" ref="Z36" si="108">X36-X35</f>
+        <v>8062</v>
+      </c>
+      <c r="AA36">
+        <f t="shared" ref="AA36" si="109">Y36-Y35</f>
+        <v>1970</v>
+      </c>
+      <c r="AB36" s="2">
+        <f t="shared" ref="AB36" si="110">AA36/Z36</f>
+        <v>0.24435623914661375</v>
+      </c>
+      <c r="AC36" s="2">
+        <f t="shared" si="103"/>
+        <v>0.23195540986952029</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <f t="shared" si="43"/>
+        <v>43940</v>
+      </c>
+      <c r="B37">
+        <v>38077</v>
+      </c>
+      <c r="C37" s="2">
+        <f t="shared" si="104"/>
+        <v>4.6876718354778399E-2</v>
+      </c>
+      <c r="D37">
+        <v>1706</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" si="96"/>
+        <v>9.358974358974359E-2</v>
+      </c>
+      <c r="F37" s="2">
+        <f t="shared" si="97"/>
+        <v>4.4803949891010324E-2</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="X37">
+        <v>162241</v>
+      </c>
+      <c r="Y37">
+        <f t="shared" si="83"/>
+        <v>38077</v>
+      </c>
+      <c r="Z37">
+        <f t="shared" ref="Z37" si="111">X37-X36</f>
+        <v>5435</v>
+      </c>
+      <c r="AA37">
+        <f t="shared" ref="AA37" si="112">Y37-Y36</f>
+        <v>1705</v>
+      </c>
+      <c r="AB37" s="2">
+        <f t="shared" ref="AB37" si="113">AA37/Z37</f>
+        <v>0.31370745170193193</v>
+      </c>
+      <c r="AC37" s="2">
+        <f t="shared" si="103"/>
+        <v>0.23469406623479885</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <f t="shared" si="43"/>
+        <v>43941</v>
+      </c>
+      <c r="B38">
+        <v>39643</v>
+      </c>
+      <c r="C38" s="2">
+        <f t="shared" si="104"/>
+        <v>4.112718964204113E-2</v>
+      </c>
+      <c r="D38">
+        <v>1809</v>
+      </c>
+      <c r="E38" s="2">
+        <f t="shared" si="96"/>
+        <v>6.0375146541617818E-2</v>
+      </c>
+      <c r="F38" s="2">
+        <f t="shared" si="97"/>
+        <v>4.5632267991827055E-2</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="99"/>
+        <v>0</v>
+      </c>
+      <c r="X38">
+        <v>169398</v>
+      </c>
+      <c r="Y38">
+        <f t="shared" si="83"/>
+        <v>39643</v>
+      </c>
+      <c r="Z38">
+        <f t="shared" ref="Z38" si="114">X38-X37</f>
+        <v>7157</v>
+      </c>
+      <c r="AA38">
+        <f t="shared" ref="AA38" si="115">Y38-Y37</f>
+        <v>1566</v>
+      </c>
+      <c r="AB38" s="2">
+        <f t="shared" ref="AB38" si="116">AA38/Z38</f>
+        <v>0.21880676261003212</v>
+      </c>
+      <c r="AC38" s="2">
+        <f t="shared" ref="AC38" si="117">Y38/X38</f>
+        <v>0.23402283379969066</v>
       </c>
     </row>
   </sheetData>

</xml_diff>